<commit_message>
latest code for TestNG
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/userInformation.xlsx
+++ b/src/test/resources/testData/userInformation.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teksc\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teksc\eclipse-workspace\tek-frameworks-testng\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6ABC060-BBF6-4A06-9C2B-9AAABE8CAF41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ABE804E-F496-445F-A5CF-8849880C8D18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{ED9F9910-2A91-4810-9BB1-032403BDE413}"/>
   </bookViews>
@@ -137,9 +137,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -458,7 +459,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="E2" sqref="E2:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -496,7 +497,7 @@
       <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
         <v>22044</v>
       </c>
     </row>
@@ -513,7 +514,7 @@
       <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="2">
         <v>22182</v>
       </c>
     </row>
@@ -530,7 +531,7 @@
       <c r="D4" t="s">
         <v>8</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="2">
         <v>22014</v>
       </c>
     </row>
@@ -547,7 +548,7 @@
       <c r="D5" t="s">
         <v>18</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="2">
         <v>11225</v>
       </c>
     </row>
@@ -564,7 +565,7 @@
       <c r="D6" t="s">
         <v>8</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="2">
         <v>22044</v>
       </c>
     </row>
@@ -581,7 +582,7 @@
       <c r="D7" t="s">
         <v>8</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="2">
         <v>22182</v>
       </c>
     </row>
@@ -598,7 +599,7 @@
       <c r="D8" t="s">
         <v>8</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="2">
         <v>22014</v>
       </c>
     </row>
@@ -615,7 +616,7 @@
       <c r="D9" t="s">
         <v>18</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="2">
         <v>11225</v>
       </c>
     </row>
@@ -632,7 +633,7 @@
       <c r="D10" t="s">
         <v>8</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="2">
         <v>22044</v>
       </c>
     </row>
@@ -649,7 +650,7 @@
       <c r="D11" t="s">
         <v>8</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="2">
         <v>22182</v>
       </c>
     </row>
@@ -666,7 +667,7 @@
       <c r="D12" t="s">
         <v>8</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="2">
         <v>22014</v>
       </c>
     </row>
@@ -683,7 +684,7 @@
       <c r="D13" t="s">
         <v>18</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="2">
         <v>11225</v>
       </c>
     </row>

</xml_diff>

<commit_message>
latest code of TestNG
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/userInformation.xlsx
+++ b/src/test/resources/testData/userInformation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teksc\eclipse-workspace\tek-frameworks-testng\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ABE804E-F496-445F-A5CF-8849880C8D18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E7B50FE-CBEC-4DE7-B94F-E2947172C093}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{ED9F9910-2A91-4810-9BB1-032403BDE413}"/>
   </bookViews>
@@ -137,10 +137,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -459,7 +458,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E13"/>
+      <selection activeCell="V12" sqref="V12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -497,7 +496,7 @@
       <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2">
         <v>22044</v>
       </c>
     </row>
@@ -514,7 +513,7 @@
       <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3">
         <v>22182</v>
       </c>
     </row>
@@ -531,7 +530,7 @@
       <c r="D4" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4">
         <v>22014</v>
       </c>
     </row>
@@ -548,7 +547,7 @@
       <c r="D5" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5">
         <v>11225</v>
       </c>
     </row>
@@ -565,7 +564,7 @@
       <c r="D6" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6">
         <v>22044</v>
       </c>
     </row>
@@ -582,7 +581,7 @@
       <c r="D7" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7">
         <v>22182</v>
       </c>
     </row>
@@ -599,7 +598,7 @@
       <c r="D8" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8">
         <v>22014</v>
       </c>
     </row>
@@ -616,7 +615,7 @@
       <c r="D9" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9">
         <v>11225</v>
       </c>
     </row>
@@ -633,7 +632,7 @@
       <c r="D10" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10">
         <v>22044</v>
       </c>
     </row>
@@ -650,7 +649,7 @@
       <c r="D11" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11">
         <v>22182</v>
       </c>
     </row>
@@ -667,7 +666,7 @@
       <c r="D12" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12">
         <v>22014</v>
       </c>
     </row>
@@ -684,7 +683,7 @@
       <c r="D13" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13">
         <v>11225</v>
       </c>
     </row>

</xml_diff>

<commit_message>
this is class code
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/userInformation.xlsx
+++ b/src/test/resources/testData/userInformation.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teksc\eclipse-workspace\tek-frameworks-testng\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E7B50FE-CBEC-4DE7-B94F-E2947172C093}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E53280C4-FBC6-4479-80A6-771C9CDC8018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{ED9F9910-2A91-4810-9BB1-032403BDE413}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" activeTab="1" xr2:uid="{ED9F9910-2A91-4810-9BB1-032403BDE413}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="5" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="26">
   <si>
     <t>name</t>
   </si>
@@ -93,6 +94,27 @@
   </si>
   <si>
     <t>Fl</t>
+  </si>
+  <si>
+    <t>cardNumber</t>
+  </si>
+  <si>
+    <t>cvcCode</t>
+  </si>
+  <si>
+    <t>nameOnCard</t>
+  </si>
+  <si>
+    <t>expirationMonth</t>
+  </si>
+  <si>
+    <t>expirationYear</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>3698521477852360</t>
   </si>
 </sst>
 </file>
@@ -137,9 +159,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -457,8 +480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDCC70BE-1620-4C7F-ABA9-ECFE17D106ED}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V12" sqref="V12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -704,4 +727,53 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A808BFEE-657A-4372-819D-2D1653DAF9C1}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>2024</v>
+      </c>
+      <c r="E2">
+        <v>145</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>